<commit_message>
Changes batch #9.1 Apr 12
</commit_message>
<xml_diff>
--- a/_dev/Examples/FBD_Tests1_Assum.xlsx
+++ b/_dev/Examples/FBD_Tests1_Assum.xlsx
@@ -14,33 +14,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve">net_speciation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time bin 1</t>
   </si>
   <si>
     <t xml:space="preserve">relative_extinction</t>
   </si>
   <si>
     <t xml:space="preserve">relative_fossilization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time bin 2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time bin 3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Time bin 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Overall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Residuals</t>
   </si>
   <si>
     <t xml:space="preserve">parameter</t>
@@ -394,29 +376,20 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-      <c r="E1" t="s">
-        <v>2</v>
+      <c r="E1" t="n">
+        <v>0.89269694921323</v>
       </c>
       <c r="F1" t="n">
-        <v>0.89269694921323</v>
-      </c>
-      <c r="G1" t="n">
         <v>0.000000000000000000000000000123318506286154</v>
       </c>
-      <c r="H1" t="s">
-        <v>1</v>
-      </c>
-      <c r="I1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" t="n">
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1" t="n">
         <v>0.612710917621017</v>
       </c>
-      <c r="K1" t="n">
+      <c r="I1" t="n">
         <v>0.000000000000000000000000000000000000000000000235567673435251</v>
-      </c>
-      <c r="L1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2">
@@ -430,31 +403,22 @@
         <v>0.000000000000000000178488253897026</v>
       </c>
       <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.911348443137957</v>
       </c>
       <c r="F2" t="n">
-        <v>0.911348443137957</v>
-      </c>
-      <c r="G2" t="n">
         <v>0.0000000000000000000000000222794575807619</v>
       </c>
-      <c r="H2" t="s">
-        <v>4</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="n">
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2" t="n">
         <v>0.878335848466453</v>
       </c>
-      <c r="K2" t="n">
+      <c r="I2" t="n">
         <v>0.00000000000000000000000000000357206584952813</v>
-      </c>
-      <c r="L2" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="3">
@@ -468,31 +432,22 @@
         <v>0.000000000000000000000000848762403275338</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.773831837183933</v>
       </c>
       <c r="F3" t="n">
-        <v>0.773831837183933</v>
-      </c>
-      <c r="G3" t="n">
         <v>0.0000000000000000000000000000000000000217874058172875</v>
       </c>
-      <c r="H3" t="s">
-        <v>5</v>
-      </c>
-      <c r="I3" t="s">
-        <v>3</v>
-      </c>
-      <c r="J3" t="n">
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3" t="n">
         <v>0.519506993796974</v>
       </c>
-      <c r="K3" t="n">
+      <c r="I3" t="n">
         <v>0.0000000000000000000000000000000000000000000000000910550848859732</v>
-      </c>
-      <c r="L3" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -506,31 +461,22 @@
         <v>0.00000000309568738124375</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.384573828801644</v>
       </c>
       <c r="F4" t="n">
-        <v>0.384573828801644</v>
-      </c>
-      <c r="G4" t="n">
         <v>0.00000000000000000000000000000000000000000000000000000771845290329158</v>
       </c>
-      <c r="H4" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" t="s">
-        <v>3</v>
-      </c>
-      <c r="J4" t="n">
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" t="n">
         <v>0.438602446305099</v>
       </c>
-      <c r="K4" t="n">
+      <c r="I4" t="n">
         <v>0.000000000000000000000000000000000000000000000000000262112010647012</v>
-      </c>
-      <c r="L4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5">
@@ -544,31 +490,22 @@
         <v>0.00000000000000000000000000000000000629965959448367</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.700783517199706</v>
       </c>
       <c r="F5" t="n">
-        <v>0.700783517199706</v>
-      </c>
-      <c r="G5" t="n">
         <v>0.00000000000000000000000000000000000000000000000000000000000000000000193136039273514</v>
       </c>
-      <c r="H5" t="s">
-        <v>7</v>
-      </c>
-      <c r="I5" t="s">
-        <v>3</v>
-      </c>
-      <c r="J5" t="n">
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" t="n">
         <v>0.554284816296558</v>
       </c>
-      <c r="K5" t="n">
+      <c r="I5" t="n">
         <v>0.0000000000000000000000000000000000000000000000000000000000000000000000000000110306675197419</v>
-      </c>
-      <c r="L5" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="6">
@@ -582,31 +519,22 @@
         <v>0.0000000000000000000871324101366285</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
-      </c>
-      <c r="E6" t="s">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.823033265753687</v>
       </c>
       <c r="F6" t="n">
-        <v>0.823033265753687</v>
-      </c>
-      <c r="G6" t="n">
         <v>0.0000000000000000000000000000000000000000000000000000000000267195077950077</v>
       </c>
-      <c r="H6" t="s">
-        <v>8</v>
-      </c>
-      <c r="I6" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" t="n">
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" t="n">
         <v>0.547685871245896</v>
       </c>
-      <c r="K6" t="n">
+      <c r="I6" t="n">
         <v>0.00000000000000000000000000000000000000000000000000000000000000000000000000000536470871005419</v>
-      </c>
-      <c r="L6" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -625,13 +553,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -647,7 +575,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>4398.87381487995</v>
@@ -658,7 +586,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>5832.15509717457</v>
@@ -683,13 +611,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>11</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2">
@@ -705,7 +633,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="n">
         <v>2942.82902209707</v>
@@ -716,7 +644,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="n">
         <v>1235.52065738462</v>

</xml_diff>